<commit_message>
Adding results of the 9n_ByStages in Folder E
</commit_message>
<xml_diff>
--- a/05. Models/06.Benchmarking/Checkpoint.xlsx
+++ b/05. Models/06.Benchmarking/Checkpoint.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\JointResearch\05. Models\06.Benchmarking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ealvarezq\Documents\GitHub\Comillas\Models\JointResearch\05. Models\06.Benchmarking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDDDB96-C15A-4DF4-8765-F8559CAC8F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77416B52-BD70-48E4-8AC8-24774A74B364}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{483A6E30-C25E-4E24-AD4C-718A8109A66F}"/>
   </bookViews>
@@ -25,10 +25,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -424,7 +424,7 @@
   <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +457,8 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -464,6 +466,8 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">

</xml_diff>